<commit_message>
update intermediate data products
</commit_message>
<xml_diff>
--- a/data/02_intermediate/stationary_guide.xlsx
+++ b/data/02_intermediate/stationary_guide.xlsx
@@ -649,7 +649,7 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
@@ -1567,7 +1567,7 @@
         <v>61</v>
       </c>
       <c r="B58">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C58" t="b">
         <v>1</v>
@@ -1584,7 +1584,7 @@
         <v>62</v>
       </c>
       <c r="B59">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C59" t="b">
         <v>1</v>
@@ -1601,7 +1601,7 @@
         <v>63</v>
       </c>
       <c r="B60">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C60" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
new intermediate data products
</commit_message>
<xml_diff>
--- a/data/02_intermediate/stationary_guide.xlsx
+++ b/data/02_intermediate/stationary_guide.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>variable</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t>ResidentialInvestment</t>
+  </si>
+  <si>
+    <t>TotalBusinessSales</t>
   </si>
   <si>
     <t>SP500</t>
@@ -587,7 +590,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1533,7 +1536,7 @@
         <v>59</v>
       </c>
       <c r="B56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C56" t="b">
         <v>1</v>
@@ -1550,7 +1553,7 @@
         <v>60</v>
       </c>
       <c r="B57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C57" t="b">
         <v>1</v>
@@ -1567,7 +1570,7 @@
         <v>61</v>
       </c>
       <c r="B58">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C58" t="b">
         <v>1</v>
@@ -1584,7 +1587,7 @@
         <v>62</v>
       </c>
       <c r="B59">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C59" t="b">
         <v>1</v>
@@ -1601,7 +1604,7 @@
         <v>63</v>
       </c>
       <c r="B60">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C60" t="b">
         <v>1</v>
@@ -1621,10 +1624,10 @@
         <v>1</v>
       </c>
       <c r="C61" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D61">
-        <v>100000000</v>
+        <v>1</v>
       </c>
       <c r="E61">
         <v>1</v>
@@ -1638,13 +1641,13 @@
         <v>1</v>
       </c>
       <c r="C62" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D62">
-        <v>1000000000</v>
+        <v>1</v>
       </c>
       <c r="E62">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1675,7 +1678,7 @@
         <v>0</v>
       </c>
       <c r="D64">
-        <v>100000000</v>
+        <v>1000000000</v>
       </c>
       <c r="E64">
         <v>4</v>
@@ -1689,13 +1692,13 @@
         <v>1</v>
       </c>
       <c r="C65" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D65">
-        <v>1</v>
+        <v>100000000</v>
       </c>
       <c r="E65">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -1746,6 +1749,23 @@
         <v>1</v>
       </c>
       <c r="E68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" t="s">
+        <v>72</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="C69" t="b">
+        <v>1</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69">
         <v>1</v>
       </c>
     </row>

</xml_diff>